<commit_message>
Modify data according to new structure of repository
</commit_message>
<xml_diff>
--- a/Planning/CM/CAR_CI_List.xlsx
+++ b/Planning/CM/CAR_CI_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>Folder</t>
   </si>
@@ -43,34 +43,10 @@
     <t>Software Requirement Specification</t>
   </si>
   <si>
-    <t>CAR_Project plan document_Vx</t>
-  </si>
-  <si>
-    <t>CAR_Requirement Traceability Matrix_Vx</t>
-  </si>
-  <si>
-    <t>CAR_Requirements_Vx</t>
-  </si>
-  <si>
-    <t>CAR_Software Interactive Questionnaire_Vx</t>
-  </si>
-  <si>
-    <t>CAR_Software Requirement Specification_Vx</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>Documents</t>
-  </si>
-  <si>
     <t>Version</t>
   </si>
   <si>
     <t>SRS is a detailed document that describes all specific requirements either function or non-function. This document according to IEEE SRS standard</t>
-  </si>
-  <si>
-    <t>CAR_Issues and Risks document_Vx</t>
   </si>
   <si>
     <t>Issues and Risks document</t>
@@ -86,12 +62,6 @@
     <t>Project Schedule </t>
   </si>
   <si>
-    <t>CAR_Project_Schedule</t>
-  </si>
-  <si>
-    <t>Version Number</t>
-  </si>
-  <si>
     <t>Implemented By</t>
   </si>
   <si>
@@ -99,12 +69,6 @@
 </t>
   </si>
   <si>
-    <t>Approved By</t>
-  </si>
-  <si>
-    <t>Approval Date</t>
-  </si>
-  <si>
     <t>Fatma mohamed</t>
   </si>
   <si>
@@ -129,9 +93,6 @@
     <t>work breakdown structure</t>
   </si>
   <si>
-    <t>CAR_work breakdown structure</t>
-  </si>
-  <si>
     <t>WBS is a key project deliverable that organizes the team's work into manageable sections</t>
   </si>
   <si>
@@ -156,9 +117,6 @@
     <t>SRS peer reviwe sheet</t>
   </si>
   <si>
-    <t>CAR_SRS_PR_Sheet</t>
-  </si>
-  <si>
     <t>A document that contains a reviewer's observations on SRS document</t>
   </si>
   <si>
@@ -166,13 +124,94 @@
   </si>
   <si>
     <t>Document contains purpose of CM, approach and Configuration Identification.</t>
+  </si>
+  <si>
+    <t>Subfolders</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Wireframe</t>
+  </si>
+  <si>
+    <t>Car_Wireframe</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>The initial design for the website</t>
+  </si>
+  <si>
+    <t>CAR_Requirements</t>
+  </si>
+  <si>
+    <t>CAR_RTM</t>
+  </si>
+  <si>
+    <t>CAR_SRS_Peer Review</t>
+  </si>
+  <si>
+    <t>CAR_SRS</t>
+  </si>
+  <si>
+    <t>CAR_Software Interactive Questionnaire</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>CAR_Issues and Risks</t>
+  </si>
+  <si>
+    <t>CAR_Project Plan _PR</t>
+  </si>
+  <si>
+    <t>Project Plan Peer Review</t>
+  </si>
+  <si>
+    <t>A document that contains a reviewer's observations on project plan document</t>
+  </si>
+  <si>
+    <t>CAR_Project_ Schedule</t>
+  </si>
+  <si>
+    <t>CAR_Risks_Peer Review</t>
+  </si>
+  <si>
+    <t>Risks Peer Review</t>
+  </si>
+  <si>
+    <t>A document that contains a reviewer's observations on Risk document</t>
+  </si>
+  <si>
+    <t>CAR_Validation &amp; Verification_Strategy</t>
+  </si>
+  <si>
+    <t>Validation &amp; Verification Strategy</t>
+  </si>
+  <si>
+    <t>CAR_WBS</t>
+  </si>
+  <si>
+    <t>CAR_Project plan document</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Reviwe Date</t>
+  </si>
+  <si>
+    <t>Reviwe By</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,14 +246,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -275,11 +306,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -287,7 +315,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -595,138 +626,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="1"/>
     <col min="2" max="2" width="33" style="1" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="50.5703125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="25.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8">
+        <v>43470</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="8">
+        <v>43501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="9">
-        <v>43470</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="9" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="9">
-        <v>43501</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -735,131 +775,178 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>33</v>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A7:A18"/>
+  <mergeCells count="3">
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" tooltip="CAR_Issues and Risks_V1.0.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_Issues and Risks_V1.0.xlsx"/>
-    <hyperlink ref="C13" r:id="rId2" tooltip="CAR_RACI.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_RACI.xlsx"/>
-    <hyperlink ref="B14" r:id="rId3" tooltip="Project Schedule Version 1.0" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/commit/18ca75c6f871fc1f88bbbc41280f7c96c4d9375a"/>
-    <hyperlink ref="C14" r:id="rId4" tooltip="CAR_Project_Schedule.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_Project_Schedule.xlsx"/>
-    <hyperlink ref="B13" r:id="rId5" tooltip="CAR_RACI.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_RACI.xlsx"/>
-    <hyperlink ref="C18" r:id="rId6" tooltip="CAR_SRS_PR_Sheet.doc" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_SRS_PR_Sheet.doc"/>
+    <hyperlink ref="B12" r:id="rId1" tooltip="CAR_Issues and Risks_V1.0.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_Issues and Risks_V1.0.xlsx"/>
+    <hyperlink ref="C14" r:id="rId2" tooltip="CAR_RACI.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_RACI.xlsx"/>
+    <hyperlink ref="B15" r:id="rId3" tooltip="Project Schedule Version 1.0" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/commit/18ca75c6f871fc1f88bbbc41280f7c96c4d9375a"/>
+    <hyperlink ref="C15" r:id="rId4" tooltip="CAR_Project_Schedule.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_Project_Schedule.xlsx"/>
+    <hyperlink ref="B14" r:id="rId5" tooltip="CAR_RACI.xlsx" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_RACI.xlsx"/>
+    <hyperlink ref="C10" r:id="rId6" tooltip="CAR_SRS_PR_Sheet.doc" display="https://github.com/FatmaMohamedSoliman/CarPurchasing/blob/Documents/CAR_SRS_PR_Sheet.doc"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>